<commit_message>
Report 09 02 2025.
</commit_message>
<xml_diff>
--- a/price_history_silver.xlsx
+++ b/price_history_silver.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="73">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -329,7 +329,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -339,10 +339,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -363,16 +359,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E138"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O82" activeCellId="0" sqref="O82"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D119" activeCellId="0" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="48.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.59"/>
   </cols>
   <sheetData>
@@ -393,877 +389,877 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="0" t="n">
         <v>2034.32</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="0" t="n">
         <v>72.66</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="0" t="n">
         <v>1816.5</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="0" t="n">
         <v>36330</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="0" t="n">
         <v>72.66</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="0" t="n">
         <v>9.08</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="0" t="n">
         <v>62.37</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="0" t="n">
         <v>62.37</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="0" t="n">
         <v>62.37</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="0" t="n">
         <v>66.6</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="0" t="n">
         <v>78.71</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="0" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="0" t="n">
         <v>64.24</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="0" t="n">
         <v>78.71</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="0" t="n">
         <v>78.71</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="0" t="n">
         <v>64.24</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="0" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="0" t="n">
         <v>64.24</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="0" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="0" t="n">
         <v>1816.5</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="0" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="0" t="n">
         <v>36330</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" s="0" t="n">
         <v>66.6</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="0" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="0" t="n">
         <v>66.6</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="0" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="0" t="n">
         <v>64.24</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="0" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" s="0" t="n">
         <v>66.6</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="0" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="0" t="n">
         <v>3571</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="3" t="n">
+      <c r="C25" s="0" t="n">
         <v>936</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="0" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="3" t="n">
+      <c r="C26" s="0" t="n">
         <v>5500</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="0" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" s="0" t="n">
         <v>5500</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="0" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="C28" s="0" t="n">
         <v>5500</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="0" t="n">
         <v>1816.5</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="0" t="n">
         <v>5607</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C31" s="0" t="n">
         <v>5304</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="0" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="3" t="n">
+      <c r="C32" s="0" t="n">
         <v>5500</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="0" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C33" s="0" t="n">
         <v>5580</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="0" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C34" s="0" t="n">
         <v>3571</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="3" t="n">
+      <c r="C35" s="0" t="n">
         <v>936</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="0" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C36" s="0" t="n">
         <v>5500</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="0" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" s="0" t="n">
         <v>5500</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="0" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C38" s="3" t="n">
+      <c r="C38" s="0" t="n">
         <v>5500</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" s="0" t="n">
         <v>1816.5</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="3" t="n">
+      <c r="C40" s="0" t="n">
         <v>5607</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="0" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
         <v>45692.9304078704</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="3" t="n">
+      <c r="C41" s="0" t="n">
         <v>5304</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="0" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B42" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B42" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="3" t="n">
+      <c r="C42" s="0" t="n">
         <v>2039.23</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B43" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B43" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="3" t="n">
+      <c r="C43" s="0" t="n">
         <v>72.84</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B44" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C44" s="3" t="n">
+      <c r="C44" s="0" t="n">
         <v>1821</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B45" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B45" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="3" t="n">
+      <c r="C45" s="0" t="n">
         <v>36420</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B46" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B46" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="3" t="n">
+      <c r="C46" s="0" t="n">
         <v>72.84</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="0" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B47" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="3" t="n">
+      <c r="C47" s="0" t="n">
         <v>9.1</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B48" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B48" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="3" t="n">
+      <c r="C48" s="0" t="n">
         <v>62.52</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="0" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B49" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B49" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="3" t="n">
+      <c r="C49" s="0" t="n">
         <v>62.52</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B50" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B50" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C50" s="3" t="n">
+      <c r="C50" s="0" t="n">
         <v>62.52</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B51" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B51" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="3" t="n">
+      <c r="C51" s="0" t="n">
         <v>66.77</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B52" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B52" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C52" s="3" t="n">
+      <c r="C52" s="0" t="n">
         <v>78.9</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="0" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B53" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B53" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="3" t="n">
+      <c r="C53" s="0" t="n">
         <v>64.4</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B54" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B54" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C54" s="3" t="n">
+      <c r="C54" s="0" t="n">
         <v>78.9</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B55" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B55" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C55" s="3" t="n">
+      <c r="C55" s="0" t="n">
         <v>78.9</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B56" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B56" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C56" s="3" t="n">
+      <c r="C56" s="0" t="n">
         <v>64.4</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="0" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B57" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B57" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C57" s="3" t="n">
+      <c r="C57" s="0" t="n">
         <v>64.4</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="0" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B58" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B58" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="3" t="n">
+      <c r="C58" s="0" t="n">
         <v>1821</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="0" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B59" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B59" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C59" s="3" t="n">
+      <c r="C59" s="0" t="n">
         <v>36420</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B60" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B60" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C60" s="3" t="n">
+      <c r="C60" s="0" t="n">
         <v>66.77</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="0" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B61" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B61" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C61" s="3" t="n">
+      <c r="C61" s="0" t="n">
         <v>66.77</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="0" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B62" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B62" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C62" s="3" t="n">
+      <c r="C62" s="0" t="n">
         <v>64.4</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="0" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
-        <v>45694.8572333963</v>
-      </c>
-      <c r="B63" s="3" t="s">
+        <v>45694.8572333912</v>
+      </c>
+      <c r="B63" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C63" s="3" t="n">
+      <c r="C63" s="0" t="n">
         <v>66.77</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="0" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>5</v>
@@ -1278,9 +1274,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>15</v>
@@ -1295,9 +1291,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>17</v>
@@ -1312,9 +1308,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>19</v>
@@ -1329,9 +1325,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>21</v>
@@ -1346,9 +1342,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>23</v>
@@ -1363,9 +1359,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>25</v>
@@ -1380,9 +1376,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>27</v>
@@ -1397,9 +1393,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>29</v>
@@ -1414,9 +1410,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>31</v>
@@ -1431,9 +1427,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>33</v>
@@ -1445,9 +1441,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>35</v>
@@ -1459,9 +1455,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>13</v>
@@ -1473,9 +1469,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>7</v>
@@ -1487,9 +1483,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>37</v>
@@ -1501,9 +1497,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>9</v>
@@ -1515,9 +1511,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B80" s="0" t="s">
         <v>39</v>
@@ -1529,9 +1525,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B81" s="0" t="s">
         <v>11</v>
@@ -1543,9 +1539,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B82" s="0" t="s">
         <v>41</v>
@@ -1557,9 +1553,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B83" s="0" t="s">
         <v>43</v>
@@ -1571,9 +1567,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B84" s="0" t="s">
         <v>45</v>
@@ -1585,9 +1581,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B85" s="0" t="s">
         <v>47</v>
@@ -1599,9 +1595,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>67</v>
@@ -1616,9 +1612,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B87" s="0" t="s">
         <v>69</v>
@@ -1633,9 +1629,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B88" s="0" t="s">
         <v>71</v>
@@ -1650,9 +1646,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B89" s="0" t="s">
         <v>67</v>
@@ -1667,9 +1663,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B90" s="0" t="s">
         <v>69</v>
@@ -1684,9 +1680,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B91" s="0" t="s">
         <v>71</v>
@@ -1701,9 +1697,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B92" s="0" t="s">
         <v>67</v>
@@ -1718,9 +1714,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>69</v>
@@ -1735,9 +1731,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="n">
-        <v>45695.8745926509</v>
+        <v>45695.8745926505</v>
       </c>
       <c r="B94" s="0" t="s">
         <v>71</v>
@@ -1750,6 +1746,682 @@
       </c>
       <c r="E94" s="0" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>2024.28</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>2582.05</v>
+      </c>
+      <c r="E95" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>2024.28</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>2582.05</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>9.04</v>
+      </c>
+      <c r="D97" s="0" t="n">
+        <v>12.06</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>9.04</v>
+      </c>
+      <c r="D98" s="0" t="n">
+        <v>12.06</v>
+      </c>
+      <c r="E98" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>62.06</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>78.86</v>
+      </c>
+      <c r="E99" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>62.06</v>
+      </c>
+      <c r="D100" s="0" t="n">
+        <v>78.86</v>
+      </c>
+      <c r="E100" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>62.06</v>
+      </c>
+      <c r="D101" s="0" t="n">
+        <v>79.58</v>
+      </c>
+      <c r="E101" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>62.06</v>
+      </c>
+      <c r="D102" s="0" t="n">
+        <v>79.58</v>
+      </c>
+      <c r="E102" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C103" s="0" t="n">
+        <v>62.06</v>
+      </c>
+      <c r="D103" s="0" t="n">
+        <v>78.86</v>
+      </c>
+      <c r="E103" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <v>62.06</v>
+      </c>
+      <c r="D104" s="0" t="n">
+        <v>78.86</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>66.28</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>115.76</v>
+      </c>
+      <c r="E105" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>66.28</v>
+      </c>
+      <c r="D106" s="0" t="n">
+        <v>115.76</v>
+      </c>
+      <c r="E106" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>78.33</v>
+      </c>
+      <c r="D107" s="0" t="n">
+        <v>173.64</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>78.33</v>
+      </c>
+      <c r="D108" s="0" t="n">
+        <v>173.64</v>
+      </c>
+      <c r="E108" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <v>63.92</v>
+      </c>
+      <c r="D109" s="0" t="n">
+        <v>153.53</v>
+      </c>
+      <c r="E109" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>63.92</v>
+      </c>
+      <c r="D110" s="0" t="n">
+        <v>153.53</v>
+      </c>
+      <c r="E110" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C111" s="0" t="n">
+        <v>78.33</v>
+      </c>
+      <c r="D111" s="0" t="n">
+        <v>173.64</v>
+      </c>
+      <c r="E111" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C112" s="0" t="n">
+        <v>78.33</v>
+      </c>
+      <c r="D112" s="0" t="n">
+        <v>173.64</v>
+      </c>
+      <c r="E112" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>78.33</v>
+      </c>
+      <c r="D113" s="0" t="n">
+        <v>202.58</v>
+      </c>
+      <c r="E113" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>78.33</v>
+      </c>
+      <c r="D114" s="0" t="n">
+        <v>202.58</v>
+      </c>
+      <c r="E114" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>63.92</v>
+      </c>
+      <c r="E115" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>63.92</v>
+      </c>
+      <c r="E116" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>63.92</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>63.92</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>72.3</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>72.3</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>72.3</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>72.3</v>
+      </c>
+      <c r="E122" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>1807.5</v>
+      </c>
+      <c r="E123" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>1807.5</v>
+      </c>
+      <c r="E124" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>1807.5</v>
+      </c>
+      <c r="E125" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <v>1807.5</v>
+      </c>
+      <c r="E126" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C127" s="0" t="n">
+        <v>36150</v>
+      </c>
+      <c r="E127" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C128" s="0" t="n">
+        <v>36150</v>
+      </c>
+      <c r="E128" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C129" s="0" t="n">
+        <v>36150</v>
+      </c>
+      <c r="E129" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C130" s="0" t="n">
+        <v>36150</v>
+      </c>
+      <c r="E130" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C131" s="0" t="n">
+        <v>66.28</v>
+      </c>
+      <c r="E131" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C132" s="0" t="n">
+        <v>66.28</v>
+      </c>
+      <c r="E132" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C133" s="0" t="n">
+        <v>66.28</v>
+      </c>
+      <c r="E133" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C134" s="0" t="n">
+        <v>66.28</v>
+      </c>
+      <c r="E134" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C135" s="0" t="n">
+        <v>63.92</v>
+      </c>
+      <c r="E135" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C136" s="0" t="n">
+        <v>63.92</v>
+      </c>
+      <c r="E136" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C137" s="0" t="n">
+        <v>66.28</v>
+      </c>
+      <c r="E137" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="2" t="n">
+        <v>45697.8568004814</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C138" s="0" t="n">
+        <v>66.28</v>
+      </c>
+      <c r="E138" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report 10 02 2025.
</commit_message>
<xml_diff>
--- a/price_history_silver.xlsx
+++ b/price_history_silver.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="73">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -359,17 +359,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E138"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D119" activeCellId="0" sqref="D119"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A144" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B163" activeCellId="0" sqref="B163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,7 +1749,7 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B95" s="0" t="s">
         <v>5</v>
@@ -1767,7 +1766,7 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B96" s="0" t="s">
         <v>5</v>
@@ -1784,7 +1783,7 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B97" s="0" t="s">
         <v>15</v>
@@ -1801,7 +1800,7 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>15</v>
@@ -1818,7 +1817,7 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>17</v>
@@ -1835,7 +1834,7 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>17</v>
@@ -1852,7 +1851,7 @@
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B101" s="0" t="s">
         <v>19</v>
@@ -1869,7 +1868,7 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B102" s="0" t="s">
         <v>19</v>
@@ -1886,7 +1885,7 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B103" s="0" t="s">
         <v>21</v>
@@ -1903,7 +1902,7 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B104" s="0" t="s">
         <v>21</v>
@@ -1920,7 +1919,7 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B105" s="0" t="s">
         <v>23</v>
@@ -1937,7 +1936,7 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B106" s="0" t="s">
         <v>23</v>
@@ -1954,7 +1953,7 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B107" s="0" t="s">
         <v>25</v>
@@ -1971,7 +1970,7 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B108" s="0" t="s">
         <v>25</v>
@@ -1988,7 +1987,7 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B109" s="0" t="s">
         <v>27</v>
@@ -2005,7 +2004,7 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>27</v>
@@ -2022,7 +2021,7 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B111" s="0" t="s">
         <v>29</v>
@@ -2039,7 +2038,7 @@
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B112" s="0" t="s">
         <v>29</v>
@@ -2056,7 +2055,7 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B113" s="0" t="s">
         <v>31</v>
@@ -2073,7 +2072,7 @@
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B114" s="0" t="s">
         <v>31</v>
@@ -2090,7 +2089,7 @@
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B115" s="0" t="s">
         <v>33</v>
@@ -2104,7 +2103,7 @@
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B116" s="0" t="s">
         <v>33</v>
@@ -2118,7 +2117,7 @@
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B117" s="0" t="s">
         <v>35</v>
@@ -2132,7 +2131,7 @@
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B118" s="0" t="s">
         <v>35</v>
@@ -2146,7 +2145,7 @@
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B119" s="0" t="s">
         <v>13</v>
@@ -2160,7 +2159,7 @@
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>13</v>
@@ -2174,7 +2173,7 @@
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B121" s="0" t="s">
         <v>7</v>
@@ -2188,7 +2187,7 @@
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B122" s="0" t="s">
         <v>7</v>
@@ -2202,7 +2201,7 @@
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B123" s="0" t="s">
         <v>37</v>
@@ -2216,7 +2215,7 @@
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B124" s="0" t="s">
         <v>37</v>
@@ -2230,7 +2229,7 @@
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B125" s="0" t="s">
         <v>9</v>
@@ -2244,7 +2243,7 @@
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B126" s="0" t="s">
         <v>9</v>
@@ -2258,7 +2257,7 @@
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B127" s="0" t="s">
         <v>39</v>
@@ -2272,7 +2271,7 @@
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B128" s="0" t="s">
         <v>39</v>
@@ -2286,7 +2285,7 @@
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>11</v>
@@ -2300,7 +2299,7 @@
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B130" s="0" t="s">
         <v>11</v>
@@ -2314,7 +2313,7 @@
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B131" s="0" t="s">
         <v>41</v>
@@ -2328,7 +2327,7 @@
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B132" s="0" t="s">
         <v>41</v>
@@ -2342,7 +2341,7 @@
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B133" s="0" t="s">
         <v>43</v>
@@ -2356,7 +2355,7 @@
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B134" s="0" t="s">
         <v>43</v>
@@ -2370,7 +2369,7 @@
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B135" s="0" t="s">
         <v>45</v>
@@ -2384,7 +2383,7 @@
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B136" s="0" t="s">
         <v>45</v>
@@ -2398,7 +2397,7 @@
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B137" s="0" t="s">
         <v>47</v>
@@ -2412,7 +2411,7 @@
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="n">
-        <v>45697.8568004814</v>
+        <v>45697.8568004861</v>
       </c>
       <c r="B138" s="0" t="s">
         <v>47</v>
@@ -2421,6 +2420,682 @@
         <v>66.28</v>
       </c>
       <c r="E138" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C139" s="0" t="n">
+        <v>2036.35</v>
+      </c>
+      <c r="D139" s="0" t="n">
+        <v>2596.87</v>
+      </c>
+      <c r="E139" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C140" s="0" t="n">
+        <v>2036.35</v>
+      </c>
+      <c r="D140" s="0" t="n">
+        <v>2596.87</v>
+      </c>
+      <c r="E140" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C141" s="0" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="D141" s="0" t="n">
+        <v>12.13</v>
+      </c>
+      <c r="E141" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C142" s="0" t="n">
+        <v>9.09</v>
+      </c>
+      <c r="D142" s="0" t="n">
+        <v>12.13</v>
+      </c>
+      <c r="E142" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C143" s="0" t="n">
+        <v>62.43</v>
+      </c>
+      <c r="D143" s="0" t="n">
+        <v>79.32</v>
+      </c>
+      <c r="E143" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C144" s="0" t="n">
+        <v>62.43</v>
+      </c>
+      <c r="D144" s="0" t="n">
+        <v>79.32</v>
+      </c>
+      <c r="E144" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C145" s="0" t="n">
+        <v>62.43</v>
+      </c>
+      <c r="D145" s="0" t="n">
+        <v>80.04</v>
+      </c>
+      <c r="E145" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C146" s="0" t="n">
+        <v>62.43</v>
+      </c>
+      <c r="D146" s="0" t="n">
+        <v>80.04</v>
+      </c>
+      <c r="E146" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C147" s="0" t="n">
+        <v>62.43</v>
+      </c>
+      <c r="D147" s="0" t="n">
+        <v>79.32</v>
+      </c>
+      <c r="E147" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C148" s="0" t="n">
+        <v>62.43</v>
+      </c>
+      <c r="D148" s="0" t="n">
+        <v>79.32</v>
+      </c>
+      <c r="E148" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C149" s="0" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="D149" s="0" t="n">
+        <v>116.42</v>
+      </c>
+      <c r="E149" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B150" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C150" s="0" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="D150" s="0" t="n">
+        <v>116.42</v>
+      </c>
+      <c r="E150" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B151" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C151" s="0" t="n">
+        <v>78.79</v>
+      </c>
+      <c r="D151" s="0" t="n">
+        <v>174.64</v>
+      </c>
+      <c r="E151" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C152" s="0" t="n">
+        <v>78.79</v>
+      </c>
+      <c r="D152" s="0" t="n">
+        <v>174.64</v>
+      </c>
+      <c r="E152" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C153" s="0" t="n">
+        <v>64.31</v>
+      </c>
+      <c r="D153" s="0" t="n">
+        <v>154.4</v>
+      </c>
+      <c r="E153" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C154" s="0" t="n">
+        <v>64.31</v>
+      </c>
+      <c r="D154" s="0" t="n">
+        <v>154.4</v>
+      </c>
+      <c r="E154" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C155" s="0" t="n">
+        <v>78.79</v>
+      </c>
+      <c r="D155" s="0" t="n">
+        <v>174.64</v>
+      </c>
+      <c r="E155" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B156" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C156" s="0" t="n">
+        <v>78.79</v>
+      </c>
+      <c r="D156" s="0" t="n">
+        <v>174.64</v>
+      </c>
+      <c r="E156" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C157" s="0" t="n">
+        <v>78.79</v>
+      </c>
+      <c r="D157" s="0" t="n">
+        <v>203.75</v>
+      </c>
+      <c r="E157" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C158" s="0" t="n">
+        <v>78.79</v>
+      </c>
+      <c r="D158" s="0" t="n">
+        <v>203.75</v>
+      </c>
+      <c r="E158" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B159" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C159" s="0" t="n">
+        <v>64.31</v>
+      </c>
+      <c r="E159" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C160" s="0" t="n">
+        <v>64.31</v>
+      </c>
+      <c r="E160" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C161" s="0" t="n">
+        <v>64.31</v>
+      </c>
+      <c r="E161" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C162" s="0" t="n">
+        <v>64.31</v>
+      </c>
+      <c r="E162" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B163" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C163" s="0" t="n">
+        <v>72.73</v>
+      </c>
+      <c r="E163" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B164" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C164" s="0" t="n">
+        <v>72.73</v>
+      </c>
+      <c r="E164" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C165" s="0" t="n">
+        <v>72.73</v>
+      </c>
+      <c r="E165" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C166" s="0" t="n">
+        <v>72.73</v>
+      </c>
+      <c r="E166" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B167" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C167" s="0" t="n">
+        <v>1818.25</v>
+      </c>
+      <c r="E167" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B168" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C168" s="0" t="n">
+        <v>1818.25</v>
+      </c>
+      <c r="E168" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C169" s="0" t="n">
+        <v>1818.25</v>
+      </c>
+      <c r="E169" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C170" s="0" t="n">
+        <v>1818.25</v>
+      </c>
+      <c r="E170" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C171" s="0" t="n">
+        <v>36365</v>
+      </c>
+      <c r="E171" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C172" s="0" t="n">
+        <v>36365</v>
+      </c>
+      <c r="E172" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C173" s="0" t="n">
+        <v>36365</v>
+      </c>
+      <c r="E173" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C174" s="0" t="n">
+        <v>36365</v>
+      </c>
+      <c r="E174" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C175" s="0" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="E175" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C176" s="0" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="E176" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C177" s="0" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="E177" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C178" s="0" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="E178" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B179" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C179" s="0" t="n">
+        <v>64.31</v>
+      </c>
+      <c r="E179" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B180" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C180" s="0" t="n">
+        <v>64.31</v>
+      </c>
+      <c r="E180" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B181" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C181" s="0" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="E181" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="2" t="n">
+        <v>45698.8279100866</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C182" s="0" t="n">
+        <v>66.67</v>
+      </c>
+      <c r="E182" s="0" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Report 13 02 2025
</commit_message>
<xml_diff>
--- a/price_history_silver.xlsx
+++ b/price_history_silver.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="67">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -341,17 +341,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E283"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A229" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A86" activeCellId="0" sqref="A86"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A250" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C276" activeCellId="0" sqref="C276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="63.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3607,7 +3606,7 @@
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B218" s="0" t="s">
         <v>5</v>
@@ -3624,7 +3623,7 @@
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B219" s="0" t="s">
         <v>5</v>
@@ -3641,7 +3640,7 @@
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B220" s="0" t="s">
         <v>15</v>
@@ -3658,7 +3657,7 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B221" s="0" t="s">
         <v>15</v>
@@ -3675,7 +3674,7 @@
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B222" s="0" t="s">
         <v>17</v>
@@ -3692,7 +3691,7 @@
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B223" s="0" t="s">
         <v>17</v>
@@ -3709,7 +3708,7 @@
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B224" s="0" t="s">
         <v>19</v>
@@ -3726,7 +3725,7 @@
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B225" s="0" t="s">
         <v>19</v>
@@ -3743,7 +3742,7 @@
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B226" s="0" t="s">
         <v>21</v>
@@ -3760,7 +3759,7 @@
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B227" s="0" t="s">
         <v>21</v>
@@ -3777,7 +3776,7 @@
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B228" s="0" t="s">
         <v>23</v>
@@ -3794,7 +3793,7 @@
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B229" s="0" t="s">
         <v>23</v>
@@ -3811,7 +3810,7 @@
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B230" s="0" t="s">
         <v>25</v>
@@ -3828,7 +3827,7 @@
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B231" s="0" t="s">
         <v>25</v>
@@ -3845,7 +3844,7 @@
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B232" s="0" t="s">
         <v>27</v>
@@ -3862,7 +3861,7 @@
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B233" s="0" t="s">
         <v>27</v>
@@ -3879,7 +3878,7 @@
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B234" s="0" t="s">
         <v>29</v>
@@ -3896,7 +3895,7 @@
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B235" s="0" t="s">
         <v>29</v>
@@ -3913,7 +3912,7 @@
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B236" s="0" t="s">
         <v>31</v>
@@ -3930,7 +3929,7 @@
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B237" s="0" t="s">
         <v>31</v>
@@ -3947,7 +3946,7 @@
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B238" s="0" t="s">
         <v>33</v>
@@ -3961,7 +3960,7 @@
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B239" s="0" t="s">
         <v>33</v>
@@ -3975,7 +3974,7 @@
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B240" s="0" t="s">
         <v>35</v>
@@ -3989,7 +3988,7 @@
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B241" s="0" t="s">
         <v>35</v>
@@ -4003,7 +4002,7 @@
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B242" s="0" t="s">
         <v>13</v>
@@ -4017,7 +4016,7 @@
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B243" s="0" t="s">
         <v>13</v>
@@ -4031,7 +4030,7 @@
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B244" s="0" t="s">
         <v>7</v>
@@ -4045,7 +4044,7 @@
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B245" s="0" t="s">
         <v>7</v>
@@ -4059,7 +4058,7 @@
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B246" s="0" t="s">
         <v>37</v>
@@ -4073,7 +4072,7 @@
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B247" s="0" t="s">
         <v>37</v>
@@ -4087,7 +4086,7 @@
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B248" s="0" t="s">
         <v>9</v>
@@ -4101,7 +4100,7 @@
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B249" s="0" t="s">
         <v>9</v>
@@ -4115,7 +4114,7 @@
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B250" s="0" t="s">
         <v>39</v>
@@ -4129,7 +4128,7 @@
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B251" s="0" t="s">
         <v>39</v>
@@ -4143,7 +4142,7 @@
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B252" s="0" t="s">
         <v>11</v>
@@ -4157,7 +4156,7 @@
     </row>
     <row r="253" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B253" s="0" t="s">
         <v>11</v>
@@ -4171,7 +4170,7 @@
     </row>
     <row r="254" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B254" s="0" t="s">
         <v>41</v>
@@ -4185,7 +4184,7 @@
     </row>
     <row r="255" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B255" s="0" t="s">
         <v>41</v>
@@ -4199,7 +4198,7 @@
     </row>
     <row r="256" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B256" s="0" t="s">
         <v>43</v>
@@ -4213,7 +4212,7 @@
     </row>
     <row r="257" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B257" s="0" t="s">
         <v>43</v>
@@ -4227,7 +4226,7 @@
     </row>
     <row r="258" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B258" s="0" t="s">
         <v>45</v>
@@ -4241,7 +4240,7 @@
     </row>
     <row r="259" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B259" s="0" t="s">
         <v>45</v>
@@ -4255,7 +4254,7 @@
     </row>
     <row r="260" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B260" s="0" t="s">
         <v>47</v>
@@ -4269,7 +4268,7 @@
     </row>
     <row r="261" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="2" t="n">
-        <v>45700.8478157995</v>
+        <v>45700.8478157986</v>
       </c>
       <c r="B261" s="0" t="s">
         <v>47</v>
@@ -4281,15 +4280,344 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B262" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C262" s="0" t="n">
+        <v>2034.37</v>
+      </c>
+      <c r="D262" s="0" t="n">
+        <v>2594.76</v>
+      </c>
+      <c r="E262" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B263" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C263" s="0" t="n">
+        <v>9.08</v>
+      </c>
+      <c r="D263" s="0" t="n">
+        <v>12.12</v>
+      </c>
+      <c r="E263" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B264" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C264" s="0" t="n">
+        <v>62.37</v>
+      </c>
+      <c r="D264" s="0" t="n">
+        <v>79.25</v>
+      </c>
+      <c r="E264" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B265" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C265" s="0" t="n">
+        <v>62.37</v>
+      </c>
+      <c r="D265" s="0" t="n">
+        <v>79.98</v>
+      </c>
+      <c r="E265" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B266" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C266" s="0" t="n">
+        <v>62.37</v>
+      </c>
+      <c r="D266" s="0" t="n">
+        <v>79.25</v>
+      </c>
+      <c r="E266" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B267" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C267" s="0" t="n">
+        <v>66.61</v>
+      </c>
+      <c r="D267" s="0" t="n">
+        <v>116.33</v>
+      </c>
+      <c r="E267" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B268" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C268" s="0" t="n">
+        <v>78.72</v>
+      </c>
+      <c r="D268" s="0" t="n">
+        <v>174.5</v>
+      </c>
+      <c r="E268" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B269" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C269" s="0" t="n">
+        <v>64.24</v>
+      </c>
+      <c r="D269" s="0" t="n">
+        <v>154.28</v>
+      </c>
+      <c r="E269" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B270" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C270" s="0" t="n">
+        <v>78.72</v>
+      </c>
+      <c r="D270" s="0" t="n">
+        <v>174.5</v>
+      </c>
+      <c r="E270" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B271" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C271" s="0" t="n">
+        <v>78.72</v>
+      </c>
+      <c r="D271" s="0" t="n">
+        <v>203.58</v>
+      </c>
+      <c r="E271" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B272" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C272" s="0" t="n">
+        <v>78.24</v>
+      </c>
+      <c r="E272" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B273" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C273" s="0" t="n">
+        <v>78.24</v>
+      </c>
+      <c r="E273" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B274" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C274" s="0" t="n">
+        <v>72.66</v>
+      </c>
+      <c r="E274" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B275" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C275" s="0" t="n">
+        <v>72.66</v>
+      </c>
+      <c r="E275" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B276" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C276" s="0" t="n">
+        <v>78.5</v>
+      </c>
+      <c r="E276" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B277" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C277" s="0" t="n">
+        <v>78.5</v>
+      </c>
+      <c r="E277" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B278" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C278" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="E278" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B279" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C279" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="E279" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B280" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C280" s="0" t="n">
+        <v>78.61</v>
+      </c>
+      <c r="E280" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B281" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C281" s="0" t="n">
+        <v>78.61</v>
+      </c>
+      <c r="E281" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B282" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C282" s="0" t="n">
+        <v>78.24</v>
+      </c>
+      <c r="E282" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="283" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="2" t="n">
+        <v>45701.8929438426</v>
+      </c>
+      <c r="B283" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C283" s="0" t="n">
+        <v>78.61</v>
+      </c>
+      <c r="E283" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>